<commit_message>
Update of documents in images, dax measures and others
</commit_message>
<xml_diff>
--- a/SQL scripts/tablas_generadas.xlsx
+++ b/SQL scripts/tablas_generadas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5075c4be90030061/Documents/Educacion/Data Analysis/Capstones Project/Personal Capstone project/Fase 2/album_financiero_phase_two/SQL scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1530" documentId="13_ncr:1_{2728BA0A-93EC-4241-81F7-DB7886A225B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80C4C505-8DA6-48B6-B2F3-E6A5DEF701ED}"/>
+  <xr:revisionPtr revIDLastSave="1542" documentId="13_ncr:1_{2728BA0A-93EC-4241-81F7-DB7886A225B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56EFFF4E-782C-413C-A87D-4E8E47DBE68C}"/>
   <bookViews>
     <workbookView xWindow="32280" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{7EB9EBB2-E148-4682-85E0-3127FDB3847D}"/>
   </bookViews>
@@ -410,30 +410,6 @@
     <t>sql_document</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>report</t>
-  </si>
-  <si>
-    <t>name_table</t>
-  </si>
-  <si>
-    <t>origin_table</t>
-  </si>
-  <si>
-    <t>meaning</t>
-  </si>
-  <si>
-    <t>columns_added_in_sql</t>
-  </si>
-  <si>
-    <t>columns_in_v_ds</t>
-  </si>
-  <si>
-    <t>columns_in_ds_for_powerbi</t>
-  </si>
-  <si>
     <t>datasets_dim</t>
   </si>
   <si>
@@ -1020,6 +996,30 @@
 categoria_ingreso
 tipo_ingreso
 canal_ingreso</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>reporte</t>
+  </si>
+  <si>
+    <t>nombre_tabla</t>
+  </si>
+  <si>
+    <t>tabla_origen</t>
+  </si>
+  <si>
+    <t>definicion</t>
+  </si>
+  <si>
+    <t>columnas_agregadas_sql</t>
+  </si>
+  <si>
+    <t>columnas_usadas_para_visualizacion</t>
+  </si>
+  <si>
+    <t>columnas_usadas_para_powerbi</t>
   </si>
 </sst>
 </file>
@@ -1450,8 +1450,8 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1468,36 +1468,36 @@
     <col min="10" max="10" width="26.7265625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>120</v>
+        <v>216</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>121</v>
+        <v>217</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>122</v>
+        <v>218</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>123</v>
+        <v>219</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>124</v>
+        <v>220</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>125</v>
+        <v>221</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>126</v>
+        <v>222</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>127</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.35">
@@ -1505,7 +1505,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>36</v>
@@ -1517,19 +1517,19 @@
         <v>92</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>93</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="96" x14ac:dyDescent="0.35">
@@ -1537,7 +1537,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>36</v>
@@ -1552,16 +1552,16 @@
         <v>57</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>96</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="132" x14ac:dyDescent="0.35">
@@ -1569,7 +1569,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>36</v>
@@ -1581,7 +1581,7 @@
         <v>70</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>49</v>
@@ -1590,10 +1590,10 @@
         <v>47</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
@@ -1601,7 +1601,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>69</v>
@@ -1613,19 +1613,19 @@
         <v>51</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>63</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="120" x14ac:dyDescent="0.35">
@@ -1633,7 +1633,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>36</v>
@@ -1645,19 +1645,19 @@
         <v>71</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1665,7 +1665,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>69</v>
@@ -1683,13 +1683,13 @@
         <v>62</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>63</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="87" x14ac:dyDescent="0.35">
@@ -1697,7 +1697,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>36</v>
@@ -1712,16 +1712,16 @@
         <v>57</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
@@ -1729,7 +1729,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>37</v>
@@ -1744,16 +1744,16 @@
         <v>9</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>63</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
@@ -1761,7 +1761,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>69</v>
@@ -1776,16 +1776,16 @@
         <v>57</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>63</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1793,7 +1793,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>36</v>
@@ -1808,7 +1808,7 @@
         <v>50</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>63</v>
@@ -1817,7 +1817,7 @@
         <v>63</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.35">
@@ -1825,7 +1825,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>36</v>
@@ -1837,19 +1837,19 @@
         <v>74</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="96" x14ac:dyDescent="0.35">
@@ -1857,7 +1857,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>69</v>
@@ -1881,7 +1881,7 @@
         <v>63</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="96" x14ac:dyDescent="0.35">
@@ -1889,7 +1889,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>69</v>
@@ -1913,7 +1913,7 @@
         <v>63</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
@@ -1921,7 +1921,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>37</v>
@@ -1939,13 +1939,13 @@
         <v>64</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>63</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="204" x14ac:dyDescent="0.35">
@@ -1953,7 +1953,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>42</v>
@@ -1965,16 +1965,16 @@
         <v>84</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>63</v>
@@ -1985,7 +1985,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>69</v>
@@ -2009,7 +2009,7 @@
         <v>63</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.35">
@@ -2017,7 +2017,7 @@
         <v>24</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>69</v>
@@ -2041,7 +2041,7 @@
         <v>63</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="120" x14ac:dyDescent="0.35">
@@ -2049,7 +2049,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>36</v>
@@ -2064,16 +2064,16 @@
         <v>57</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2081,7 +2081,7 @@
         <v>27</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>69</v>
@@ -2099,13 +2099,13 @@
         <v>100</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>63</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="84" x14ac:dyDescent="0.35">
@@ -2113,7 +2113,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>69</v>
@@ -2137,7 +2137,7 @@
         <v>63</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="144" x14ac:dyDescent="0.35">
@@ -2145,7 +2145,7 @@
         <v>31</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>37</v>
@@ -2160,16 +2160,16 @@
         <v>0</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>63</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="145.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2177,7 +2177,7 @@
         <v>33</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>37</v>
@@ -2192,16 +2192,16 @@
         <v>6</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>63</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="108" x14ac:dyDescent="0.35">
@@ -2209,7 +2209,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>37</v>
@@ -2227,13 +2227,13 @@
         <v>65</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>63</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2241,7 +2241,7 @@
         <v>35</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>69</v>
@@ -2273,7 +2273,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>36</v>
@@ -2285,19 +2285,19 @@
         <v>76</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2305,7 +2305,7 @@
         <v>41</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>69</v>
@@ -2337,7 +2337,7 @@
         <v>43</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>36</v>
@@ -2349,19 +2349,19 @@
         <v>77</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -2369,7 +2369,7 @@
         <v>88</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>69</v>
@@ -2401,7 +2401,7 @@
         <v>97</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>69</v>
@@ -2419,13 +2419,13 @@
         <v>99</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>63</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -2433,7 +2433,7 @@
         <v>102</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>69</v>
@@ -2465,7 +2465,7 @@
         <v>106</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>36</v>
@@ -2480,16 +2480,16 @@
         <v>57</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
@@ -2497,7 +2497,7 @@
         <v>109</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>69</v>
@@ -2529,7 +2529,7 @@
         <v>113</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>69</v>
@@ -2561,7 +2561,7 @@
         <v>117</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>36</v>
@@ -2573,27 +2573,27 @@
         <v>118</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>69</v>
@@ -2602,13 +2602,13 @@
         <v>14</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>71</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>63</v>
@@ -2617,15 +2617,15 @@
         <v>63</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>69</v>
@@ -2634,13 +2634,13 @@
         <v>38</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>57</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>63</v>
@@ -2654,10 +2654,10 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>69</v>
@@ -2666,13 +2666,13 @@
         <v>107</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>108</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>63</v>
@@ -2681,7 +2681,7 @@
         <v>63</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>